<commit_message>
Dropdown made in board!!!
</commit_message>
<xml_diff>
--- a/Project2017/Overige bestanden/index.xlsx
+++ b/Project2017/Overige bestanden/index.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\looij\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documenten\Programming\git\Project2017\Project2017\Overige bestanden\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -412,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,12 +423,12 @@
     <col min="8" max="8" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>0</v>
       </c>
@@ -442,7 +442,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -465,7 +465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -489,7 +489,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -513,7 +513,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -530,12 +530,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -552,7 +552,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -569,7 +569,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -586,7 +586,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
@@ -603,12 +603,24 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>25</v>
+      </c>
+      <c r="K16">
+        <v>2</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -624,8 +636,20 @@
       <c r="E17" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>44</v>
+      </c>
+      <c r="K17">
+        <v>3</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -642,7 +666,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -658,8 +682,20 @@
       <c r="E19" s="1">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <v>18</v>
+      </c>
+      <c r="K19">
+        <v>2</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -676,12 +712,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -698,7 +734,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -715,7 +751,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
@@ -732,7 +768,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Development of BoardTest and creation of FieldNotExsistException
</commit_message>
<xml_diff>
--- a/Project2017/Overige bestanden/index.xlsx
+++ b/Project2017/Overige bestanden/index.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documenten\Programming\git\Project2017\Project2017\Overige bestanden\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\looij\git\Project2017\Project2017\Overige bestanden\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>DIM</t>
   </si>
@@ -46,6 +46,9 @@
   <si>
     <t>y=3</t>
   </si>
+  <si>
+    <t>TEST</t>
+  </si>
 </sst>
 </file>
 
@@ -60,12 +63,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -95,9 +110,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -415,7 +432,7 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,6 +551,12 @@
       <c r="C9" t="s">
         <v>5</v>
       </c>
+      <c r="H9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -551,6 +574,10 @@
       <c r="E10" s="1">
         <v>35</v>
       </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -568,6 +595,10 @@
       <c r="E11" s="1">
         <v>39</v>
       </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -585,6 +616,10 @@
       <c r="E12" s="1">
         <v>43</v>
       </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -601,24 +636,28 @@
       </c>
       <c r="E13" s="1">
         <v>47</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>4</v>
       </c>
-      <c r="J16">
-        <v>25</v>
-      </c>
-      <c r="K16">
-        <v>2</v>
-      </c>
-      <c r="L16">
-        <v>1</v>
-      </c>
-      <c r="M16">
-        <v>1</v>
-      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="3"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -636,18 +675,13 @@
       <c r="E17" s="1">
         <v>19</v>
       </c>
-      <c r="J17">
-        <v>44</v>
-      </c>
-      <c r="K17">
-        <v>3</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>2</v>
-      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17" s="3"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="1"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -665,6 +699,13 @@
       <c r="E18" s="1">
         <v>23</v>
       </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+      <c r="J18" s="1"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="1"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -682,18 +723,13 @@
       <c r="E19" s="1">
         <v>27</v>
       </c>
-      <c r="J19">
-        <v>18</v>
-      </c>
-      <c r="K19">
-        <v>2</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>1</v>
-      </c>
+      <c r="I19">
+        <v>3</v>
+      </c>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -710,6 +746,18 @@
       </c>
       <c r="E20" s="1">
         <v>31</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>2</v>
+      </c>
+      <c r="M20">
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>